<commit_message>
Actually don't know it just changed
</commit_message>
<xml_diff>
--- a/Risikoannalyse_TerminprosjektVG2_Peder.xlsx
+++ b/Risikoannalyse_TerminprosjektVG2_Peder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/pehaa002_osloskolen_no/Documents/Kuben/VG2/IM/Terminprosjekt/Terminprosjekt_VG2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F48F640-A146-4887-A29D-1B39F9790BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{5F48F640-A146-4887-A29D-1B39F9790BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA85983F-4803-4691-8EB1-72F9E719B36A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4F7841C-9437-411E-AE34-9396186903BB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A4F7841C-9437-411E-AE34-9396186903BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,13 +633,13 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="71.5546875" bestFit="1" customWidth="1"/>

</xml_diff>